<commit_message>
Updated the configfile and added log messages before and after each flows for monitoring.
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://reedelsevier-my.sharepoint.com/personal/rollle01_risk_regn_net/Documents/Documents/UiPath/FLRenamingAutomationFinal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{6419CE06-BB56-4160-8377-4E4AD514CD23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A0B000CB-C101-4940-8233-0685AFD4DC41}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D2A51F-33C1-4994-BBC6-FC2CCB2A86C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
+    <sheet name="ConfigOptions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -47,56 +48,122 @@
     <t>Description</t>
   </si>
   <si>
-    <t>MasterFile</t>
-  </si>
-  <si>
-    <t>"C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\FLOBOT\" &amp; Date.Now.ToString("MMddyyyy") &amp; "\" &amp; Date.Now.ToString("MMddyyyy") &amp; ".xlsx"</t>
-  </si>
-  <si>
-    <t>FlobotFolder</t>
-  </si>
-  <si>
-    <t>"C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\FLOBOT\" &amp; Date.Now.ToString("MMddyyyy")</t>
-  </si>
-  <si>
-    <t>FlobotSubFolder</t>
-  </si>
-  <si>
-    <t>FlobotFolder &amp; "\RAW FL FILES"</t>
-  </si>
-  <si>
-    <t>Specific folder where raw files for renaming are saved</t>
-  </si>
-  <si>
-    <t>DoneFolder</t>
-  </si>
-  <si>
-    <t>Path.Combine(FlobotFolder, "DONE")</t>
-  </si>
-  <si>
-    <t>Folder where renamed files are saved</t>
-  </si>
-  <si>
     <t>DeleteDirectory</t>
   </si>
   <si>
-    <t>"C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\FLOBOT"</t>
-  </si>
-  <si>
     <t>Directory to be scanned for files that are older than 90 days.</t>
   </si>
   <si>
-    <t>File where transaction and report numbers are stored. It is also being updated once the automation run is completed.</t>
-  </si>
-  <si>
-    <t>Folder with today's date where PDF files and masterfile for processing are saved.</t>
+    <t>BaseURL</t>
+  </si>
+  <si>
+    <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\FLOBOT</t>
+  </si>
+  <si>
+    <t>SuffixDone</t>
+  </si>
+  <si>
+    <t>SuffixToday</t>
+  </si>
+  <si>
+    <t>%2FDONE&amp;viewid=0cafe987%2D9ce0%2D4c52%2Dbaeb%2D28681de003dc</t>
+  </si>
+  <si>
+    <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\FLOBOT\</t>
+  </si>
+  <si>
+    <t>SharePoint site's FLOBOT folder - base URL</t>
+  </si>
+  <si>
+    <t>SharePoint site's FLOBOT DONE folder</t>
+  </si>
+  <si>
+    <t>SharePoint site's FLOBOT folder - suffix URL (after current date)</t>
+  </si>
+  <si>
+    <t>https://reedelsevier.sharepoint.com/sites/RollanLester/Shared%20Documents/Forms/AllItems.aspx?id=%2Fsites%2FRollanLester%2FShared%20Documents%2FFLOBOT%2F</t>
+  </si>
+  <si>
+    <t>%2FDONE&amp;viewid=105abaaa%2D085a%2D4a79%2D8458%2D7b6ecbd5487b</t>
+  </si>
+  <si>
+    <t>TempFiles</t>
+  </si>
+  <si>
+    <t>crdownload, part, tmp, download, filepart, txt, log</t>
+  </si>
+  <si>
+    <t>Main folder where today's transactions to be processed are saved</t>
+  </si>
+  <si>
+    <t>temporary files that should be ignored for the wait for download activity</t>
+  </si>
+  <si>
+    <t>MasterFolder</t>
+  </si>
+  <si>
+    <t>ZippedDirectory</t>
+  </si>
+  <si>
+    <t>C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Desktop\FLOBOT</t>
+  </si>
+  <si>
+    <t>Zipped folder directory</t>
+  </si>
+  <si>
+    <t>ROLLLE01 SP to Local Computer - Testing</t>
+  </si>
+  <si>
+    <t>FLOBOT SP to Local Computer - Testing</t>
+  </si>
+  <si>
+    <t>https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F</t>
+  </si>
+  <si>
+    <t>FLOBOT SP to Virtual Desktop - Testing</t>
+  </si>
+  <si>
+    <t>appmail.risk.regn.net</t>
+  </si>
+  <si>
+    <t>Virtual desktop's email server</t>
+  </si>
+  <si>
+    <t>SMTPServer</t>
+  </si>
+  <si>
+    <t>RecipientTo</t>
+  </si>
+  <si>
+    <t>RecipientCC</t>
+  </si>
+  <si>
+    <t>sam.tecson@lexisnexisrisk.com; joavic.quisano@lexisnexisrisk.com</t>
+  </si>
+  <si>
+    <t>lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; jhoanna.talle@lexisnexisrisk.com</t>
+  </si>
+  <si>
+    <t>To List</t>
+  </si>
+  <si>
+    <t>CC List</t>
+  </si>
+  <si>
+    <t>E:\Bot_Files\RPA FL Renaming\FLOBOT\</t>
+  </si>
+  <si>
+    <t>E:\Bot_Files\RPA FL Renaming\FLOBOT</t>
+  </si>
+  <si>
+    <t>sam.tecson@lexisnexisrisk.com; joavic.quisano@lexisnexisrisk.com; david.villasoto@lexisnexisrisk.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -112,13 +179,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF002060"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -130,10 +218,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -147,8 +236,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,18 +577,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FCB039-29A7-49D1-BD2D-CAC9DFC1D441}">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.90625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="20.81640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="77.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="45.08984375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="32.90625" style="2"/>
+    <col min="3" max="3" width="45.1796875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="32.81640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -506,26 +602,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
+      <c r="B3" s="5" t="s">
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
@@ -533,58 +629,88 @@
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
@@ -621,32 +747,434 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{A126A96C-2DAA-4BEB-B2AD-B554B4E4A65A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
+  <dimension ref="A1:C40"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="78.81640625" customWidth="1"/>
+    <col min="3" max="3" width="64.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A29:C29"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{44FFA718-53D0-4FDC-954B-616ACF922B74}"/>
+    <hyperlink ref="B18" r:id="rId2" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{61DFF7CE-7C20-423C-8D48-22C4B19EAF6B}"/>
+    <hyperlink ref="B32" r:id="rId3" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{75507591-B60F-4C09-AA68-537942F695CD}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated the configfile for the To and CC list in the auto-email notification.
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4D2A51F-33C1-4994-BBC6-FC2CCB2A86C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1331B7-D587-45B2-AA4D-8A2A177D81E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>RecipientCC</t>
-  </si>
-  <si>
-    <t>sam.tecson@lexisnexisrisk.com; joavic.quisano@lexisnexisrisk.com</t>
   </si>
   <si>
     <t>lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; jhoanna.talle@lexisnexisrisk.com</t>
@@ -579,19 +576,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FCB039-29A7-49D1-BD2D-CAC9DFC1D441}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="77.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="45.1796875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="32.81640625" style="2"/>
+    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="32.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -602,18 +599,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>37</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -624,7 +621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -635,7 +632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -646,18 +643,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -668,18 +665,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -690,66 +687,66 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{A126A96C-2DAA-4BEB-B2AD-B554B4E4A65A}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{AE603AE5-8317-43DD-94B6-FAA4A34FF1BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -759,25 +756,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C26"/>
+    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39:B40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="78.81640625" customWidth="1"/>
-    <col min="3" max="3" width="64.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="78.85546875" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -788,7 +785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -799,7 +796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -810,7 +807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -821,7 +818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -832,7 +829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -843,7 +840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -854,7 +851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -865,7 +862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -876,46 +873,46 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -926,7 +923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -937,7 +934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -948,7 +945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -959,7 +956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -970,7 +967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -981,7 +978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -992,7 +989,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1003,7 +1000,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1014,36 +1011,36 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>0</v>
       </c>
@@ -1054,18 +1051,18 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1076,7 +1073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1087,7 +1084,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -1098,18 +1095,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1120,18 +1117,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
@@ -1142,26 +1139,26 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated ConfigFile (To and CC list) for testing in Orchestrator.
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1331B7-D587-45B2-AA4D-8A2A177D81E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792CEFF9-CE2D-45E1-881E-D2FB40BC00C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -138,9 +138,6 @@
     <t>RecipientCC</t>
   </si>
   <si>
-    <t>lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; jhoanna.talle@lexisnexisrisk.com</t>
-  </si>
-  <si>
     <t>To List</t>
   </si>
   <si>
@@ -154,6 +151,12 @@
   </si>
   <si>
     <t>sam.tecson@lexisnexisrisk.com; joavic.quisano@lexisnexisrisk.com; david.villasoto@lexisnexisrisk.com</t>
+  </si>
+  <si>
+    <t>lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; jhoanna.talle@lexisnexisrisk.com; paul.fabro@lexisnexisrisk.com; judy.cotaoco@lexisnexisrisk.com</t>
+  </si>
+  <si>
+    <t>lester.rollan@lexisnexisrisk.com</t>
   </si>
 </sst>
 </file>
@@ -604,7 +607,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -648,7 +651,7 @@
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
@@ -670,7 +673,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
@@ -687,26 +690,26 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -756,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:B40"/>
+    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -878,21 +881,21 @@
         <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1016,21 +1019,21 @@
         <v>31</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
@@ -1056,7 +1059,7 @@
         <v>3</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>4</v>
@@ -1100,7 +1103,7 @@
         <v>20</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>18</v>
@@ -1122,7 +1125,7 @@
         <v>21</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>23</v>
@@ -1144,21 +1147,21 @@
         <v>31</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the configfile and file download flow for testing.
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{792CEFF9-CE2D-45E1-881E-D2FB40BC00C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2A998C-AAD7-4AD6-B6EE-47C42E5E75DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,8 +759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:C38"/>
+    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Updated the ConfigFile and adjusted the delays within the SharePoint download workflow after testing.
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE2A998C-AAD7-4AD6-B6EE-47C42E5E75DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C220CBAB-32CC-48E2-A461-A7B91A4299DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
   <si>
     <t>Name</t>
   </si>
@@ -154,9 +154,6 @@
   </si>
   <si>
     <t>lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; jhoanna.talle@lexisnexisrisk.com; paul.fabro@lexisnexisrisk.com; judy.cotaoco@lexisnexisrisk.com</t>
-  </si>
-  <si>
-    <t>lester.rollan@lexisnexisrisk.com</t>
   </si>
 </sst>
 </file>
@@ -580,7 +577,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,23 +687,23 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>34</v>
@@ -760,7 +757,7 @@
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B37"/>
+      <selection activeCell="B39" sqref="B39:B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added "Element Exists" activity in the "SharePoint download" workflow
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C220CBAB-32CC-48E2-A461-A7B91A4299DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41619E27-67C9-4AA1-AF0F-3715E9074F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -577,18 +577,18 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B11"/>
+      <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="77.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="32.85546875" style="2"/>
+    <col min="1" max="1" width="20.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="77.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.1796875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="32.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -599,7 +599,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -610,7 +610,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -621,7 +621,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -632,7 +632,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -643,7 +643,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -654,7 +654,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -665,7 +665,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -676,7 +676,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -687,7 +687,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -698,7 +698,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -709,37 +709,37 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -756,25 +756,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39:B40"/>
+    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35:B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="78.85546875" customWidth="1"/>
-    <col min="3" max="3" width="64.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="78.81640625" customWidth="1"/>
+    <col min="3" max="3" width="64.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -785,7 +785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -796,7 +796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -807,7 +807,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -818,7 +818,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -829,7 +829,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -840,7 +840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -851,7 +851,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -862,7 +862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -873,7 +873,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -884,7 +884,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -895,24 +895,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -923,7 +923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -934,7 +934,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -945,7 +945,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -956,7 +956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -967,7 +967,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -978,7 +978,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -989,7 +989,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1000,7 +1000,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1011,7 +1011,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1022,7 +1022,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1033,14 +1033,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1073,7 +1073,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1084,7 +1084,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -1095,7 +1095,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -1106,7 +1106,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1117,7 +1117,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
@@ -1150,7 +1150,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Updated the following before uploading a new package to Orchestartor: - Revise the message in the post automation email. - Adjusted the kill process activity before the sharepoint download workflow. - Added an "Element Exists" activity before saving the zipped folder - Adjusted the ConfigFile for testing
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41619E27-67C9-4AA1-AF0F-3715E9074F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E78149-874F-4DEA-860D-BAC27607AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
+    <workbookView xWindow="12690" yWindow="-630" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
   <si>
     <t>Name</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; jhoanna.talle@lexisnexisrisk.com; paul.fabro@lexisnexisrisk.com; judy.cotaoco@lexisnexisrisk.com</t>
+  </si>
+  <si>
+    <t>lester.rollan@lexisnexisrisk.com</t>
   </si>
 </sst>
 </file>
@@ -576,19 +579,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FCB039-29A7-49D1-BD2D-CAC9DFC1D441}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="77.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="45.1796875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="32.81640625" style="2"/>
+    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="32.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -599,7 +602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -610,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -621,7 +624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -632,7 +635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -643,7 +646,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -654,7 +657,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -665,7 +668,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -676,7 +679,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -687,59 +690,59 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -756,25 +759,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B35" sqref="B35:B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="78.81640625" customWidth="1"/>
-    <col min="3" max="3" width="64.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="78.85546875" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -785,7 +788,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -796,7 +799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -807,7 +810,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -818,7 +821,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -829,7 +832,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -840,7 +843,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -851,7 +854,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -862,7 +865,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -873,7 +876,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -884,7 +887,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -895,24 +898,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -923,7 +926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -934,7 +937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -945,7 +948,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -956,7 +959,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -967,7 +970,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -978,7 +981,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -989,7 +992,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1000,7 +1003,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1011,7 +1014,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1022,7 +1025,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1033,14 +1036,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -1062,7 +1065,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1073,7 +1076,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1084,7 +1087,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -1095,7 +1098,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -1106,7 +1109,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1117,7 +1120,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -1128,7 +1131,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
@@ -1150,7 +1153,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Edited the selectors in the "Element Exists" activities for downloading and saving zipped files.
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E78149-874F-4DEA-860D-BAC27607AACB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6F3277-ED46-40A0-9A72-221110800247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12690" yWindow="-630" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
@@ -580,7 +580,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B6" sqref="B6:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,7 +759,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B35" sqref="B35:B37"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated ConfigFile and selector when downloading files in SharePoint folder.
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D6F3277-ED46-40A0-9A72-221110800247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61209AA5-E4C9-4184-96EE-01FF80D856C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12690" yWindow="-630" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -580,18 +580,18 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="77.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="32.85546875" style="2"/>
+    <col min="1" max="1" width="20.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="77.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.1796875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="32.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -602,7 +602,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -613,7 +613,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -624,7 +624,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -635,7 +635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -646,18 +646,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>35</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -668,18 +668,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -690,59 +690,59 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>39</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -750,6 +750,8 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{AE603AE5-8317-43DD-94B6-FAA4A34FF1BA}"/>
+    <hyperlink ref="B11" r:id="rId2" xr:uid="{B2F6CD77-8A2C-40E9-B3B6-54835E63E71B}"/>
+    <hyperlink ref="B10" r:id="rId3" xr:uid="{9DFCC8BD-25D8-4A97-8A1D-E7C7BCC1CAAF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -759,25 +761,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:B37"/>
+    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="78.85546875" customWidth="1"/>
-    <col min="3" max="3" width="64.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="78.81640625" customWidth="1"/>
+    <col min="3" max="3" width="64.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -788,7 +790,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -799,7 +801,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -810,7 +812,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -821,7 +823,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -832,7 +834,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -843,7 +845,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -854,7 +856,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -865,7 +867,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -876,7 +878,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -887,7 +889,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -898,24 +900,24 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>0</v>
       </c>
@@ -926,7 +928,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>3</v>
       </c>
@@ -937,7 +939,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
@@ -948,7 +950,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>7</v>
       </c>
@@ -959,7 +961,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -970,7 +972,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -981,7 +983,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>16</v>
       </c>
@@ -992,7 +994,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -1003,7 +1005,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>30</v>
       </c>
@@ -1014,7 +1016,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>31</v>
       </c>
@@ -1025,7 +1027,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>32</v>
       </c>
@@ -1036,14 +1038,14 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A29" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="6"/>
       <c r="C29" s="6"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1056,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>3</v>
       </c>
@@ -1065,7 +1067,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>5</v>
       </c>
@@ -1076,7 +1078,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>7</v>
       </c>
@@ -1087,7 +1089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>8</v>
       </c>
@@ -1098,7 +1100,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>20</v>
       </c>
@@ -1109,7 +1111,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>16</v>
       </c>
@@ -1120,7 +1122,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>21</v>
       </c>
@@ -1131,7 +1133,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>30</v>
       </c>
@@ -1142,7 +1144,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>31</v>
       </c>
@@ -1153,7 +1155,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Updates done: - flow updated for the downloaded files to be saved in the default "Downloads" folder - flow updated for the downloaded files from the "Downloads" folder to be moved to the MasterFolder
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61209AA5-E4C9-4184-96EE-01FF80D856C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDEA640-0F68-4C32-B1CF-F3D49E0D297C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="43">
   <si>
     <t>Name</t>
   </si>
@@ -156,7 +156,16 @@
     <t>lester.rollan@lexisnexisrisk.com; dindee.galindo@lexisnexisrisk.com; jesriel.tolentino@lexisnexisrisk.com; jhoanna.talle@lexisnexisrisk.com; paul.fabro@lexisnexisrisk.com; judy.cotaoco@lexisnexisrisk.com</t>
   </si>
   <si>
-    <t>lester.rollan@lexisnexisrisk.com</t>
+    <t>DownloadsFolder</t>
+  </si>
+  <si>
+    <t>C:\Users\RollLe01\Downloads\</t>
+  </si>
+  <si>
+    <t>Download folder's path</t>
+  </si>
+  <si>
+    <t>C:\Users\svc-RCOUIPBOT0005\Downloads\</t>
   </si>
 </sst>
 </file>
@@ -579,19 +588,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FCB039-29A7-49D1-BD2D-CAC9DFC1D441}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.81640625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="77.453125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="45.1796875" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="32.81640625" style="2"/>
+    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="77.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.140625" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="32.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -602,7 +611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -613,7 +622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -624,7 +633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -635,7 +644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -646,18 +655,18 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -668,18 +677,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -690,68 +699,72 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>39</v>
+      <c r="B10" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>39</v>
+      <c r="B11" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{AE603AE5-8317-43DD-94B6-FAA4A34FF1BA}"/>
-    <hyperlink ref="B11" r:id="rId2" xr:uid="{B2F6CD77-8A2C-40E9-B3B6-54835E63E71B}"/>
-    <hyperlink ref="B10" r:id="rId3" xr:uid="{9DFCC8BD-25D8-4A97-8A1D-E7C7BCC1CAAF}"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{AD483FD3-D015-4425-8DAF-68CF9AB1E593}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -759,27 +772,27 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
-  <dimension ref="A1:C40"/>
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:B26"/>
+    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.1796875" customWidth="1"/>
-    <col min="2" max="2" width="78.81640625" customWidth="1"/>
-    <col min="3" max="3" width="64.1796875" customWidth="1"/>
+    <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="78.85546875" customWidth="1"/>
+    <col min="3" max="3" width="64.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -790,7 +803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -801,7 +814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -812,7 +825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -823,7 +836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -834,7 +847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -845,7 +858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -856,7 +869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -867,7 +880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -878,7 +891,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -889,7 +902,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -900,282 +913,315 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="6" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B17" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C17" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C19" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="1" t="s">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="1" t="s">
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="1" t="s">
+      <c r="C23" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B24" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B25" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C25" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C26" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B27" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="6" t="s">
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="1" t="s">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B33" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="1" t="s">
+    <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A33" s="1" t="s">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C35" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A34" s="1" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B36" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C34" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A35" s="1" t="s">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B37" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C35" s="1" t="s">
+      <c r="C37" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A36" s="1" t="s">
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B38" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C36" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A37" s="1" t="s">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A38" s="1" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B40" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="29" x14ac:dyDescent="0.35">
-      <c r="A39" s="1" t="s">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A40" s="1" t="s">
+    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B42" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C40" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>34</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A15:C15"/>
-    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A31:C31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{44FFA718-53D0-4FDC-954B-616ACF922B74}"/>
-    <hyperlink ref="B18" r:id="rId2" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{61DFF7CE-7C20-423C-8D48-22C4B19EAF6B}"/>
-    <hyperlink ref="B32" r:id="rId3" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{75507591-B60F-4C09-AA68-537942F695CD}"/>
+    <hyperlink ref="B19" r:id="rId2" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{61DFF7CE-7C20-423C-8D48-22C4B19EAF6B}"/>
+    <hyperlink ref="B34" r:id="rId3" display="https://reedelsevier.sharepoint.com/sites/OG-ONECRUIR/Shared%20Documents/Forms/AllItems.aspx?newTargetListUrl=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents&amp;viewpath=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FForms%2FAllItems%2Easpx&amp;id=%2Fsites%2FOG%2DONECRUIR%2FShared%20Documents%2FFLOBOT%2F" xr:uid="{75507591-B60F-4C09-AA68-537942F695CD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated the selectors in searching and clicking the folder with today's date
</commit_message>
<xml_diff>
--- a/FLRenamingConfigFile.xlsx
+++ b/FLRenamingConfigFile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RollLe01\OneDrive - Reed Elsevier Group ICO Reed Elsevier Inc\Documents\UiPath\FLRenamingAutomationFinal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDEA640-0F68-4C32-B1CF-F3D49E0D297C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E43E2AE0-8907-4B09-B85A-96FBDA512DFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{42A39E5C-086F-4F21-8E01-13B402E1EF9B}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
@@ -588,19 +588,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44FCB039-29A7-49D1-BD2D-CAC9DFC1D441}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="32.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="32.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="77.42578125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="45.140625" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="32.85546875" style="2"/>
+    <col min="1" max="1" width="20.81640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="77.453125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="45.1796875" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="32.81640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -611,7 +611,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
@@ -622,7 +622,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -633,7 +633,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -644,7 +644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -655,7 +655,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -666,7 +666,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>16</v>
       </c>
@@ -677,7 +677,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
@@ -688,7 +688,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
@@ -699,7 +699,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>31</v>
       </c>
@@ -710,7 +710,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>32</v>
       </c>
@@ -721,7 +721,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>39</v>
       </c>
@@ -732,32 +732,32 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -774,25 +774,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76F6061F-8D4B-4607-9BDC-CC06CA27F46E}">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37:B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.140625" customWidth="1"/>
-    <col min="2" max="2" width="78.85546875" customWidth="1"/>
-    <col min="3" max="3" width="64.140625" customWidth="1"/>
+    <col min="1" max="1" width="15.1796875" customWidth="1"/>
+    <col min="2" max="2" width="78.81640625" customWidth="1"/>
+    <col min="3" max="3" width="64.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>24</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -803,7 +803,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -814,7 +814,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -825,7 +825,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
@@ -836,7 +836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>8</v>
       </c>
@@ -847,7 +847,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
@@ -858,7 +858,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -869,7 +869,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -880,7 +880,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>30</v>
       </c>
@@ -891,7 +891,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>31</v>
       </c>
@@ -902,7 +902,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -913,7 +913,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -924,24 +924,24 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="6" t="s">
         <v>25</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>0</v>
       </c>
@@ -952,7 +952,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>3</v>
       </c>
@@ -963,7 +963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
@@ -974,7 +974,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
@@ -985,7 +985,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -996,7 +996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -1007,7 +1007,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>16</v>
       </c>
@@ -1018,7 +1018,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>21</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>30</v>
       </c>
@@ -1040,7 +1040,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>31</v>
       </c>
@@ -1051,7 +1051,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>32</v>
       </c>
@@ -1062,7 +1062,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>39</v>
       </c>
@@ -1073,14 +1073,14 @@
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="6" t="s">
         <v>27</v>
       </c>
       <c r="B31" s="6"/>
       <c r="C31" s="6"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
         <v>0</v>
       </c>
@@ -1091,7 +1091,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -1102,7 +1102,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>5</v>
       </c>
@@ -1113,7 +1113,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>7</v>
       </c>
@@ -1124,7 +1124,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>8</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>20</v>
       </c>
@@ -1146,7 +1146,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>16</v>
       </c>
@@ -1157,7 +1157,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>21</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>30</v>
       </c>
@@ -1179,7 +1179,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>31</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>32</v>
       </c>
@@ -1201,7 +1201,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>39</v>
       </c>

</xml_diff>